<commit_message>
edit in upload functions of overnightdays
</commit_message>
<xml_diff>
--- a/excelforms/نوباتجية.xlsx
+++ b/excelforms/نوباتجية.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\payroll\excelforms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658F205F-D7EF-4E0B-B60E-985DC3D9D5DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32A2EF7-E48F-4901-8E9F-E1ABB6D1DF1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,9 +109,7 @@
     <tableColumn id="1" xr3:uid="{E18AD355-88EB-46C2-A57C-A710F528C13F}" name="رقم القيد"/>
     <tableColumn id="2" xr3:uid="{6123294E-83E4-4232-9ADB-4F0873F170E2}" name="الاسم"/>
     <tableColumn id="3" xr3:uid="{9E062A66-EB9E-4833-821A-4607D845A9F4}" name="الحضـور"/>
-    <tableColumn id="4" xr3:uid="{F2E4ED7C-17EF-4D2F-9B80-651A45868C8A}" name="الايام المستحقة">
-      <calculatedColumnFormula>Table1[[#This Row],[الحضـور]]*2</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="4" xr3:uid="{F2E4ED7C-17EF-4D2F-9B80-651A45868C8A}" name="الايام المستحقة"/>
     <tableColumn id="5" xr3:uid="{44D30526-ABAC-495D-AEDF-0AC06193C2EC}" name="ملاحظات"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -384,7 +382,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +418,6 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <f>Table1[[#This Row],[الحضـور]]*2</f>
         <v>2</v>
       </c>
     </row>
@@ -432,7 +429,6 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <f>Table1[[#This Row],[الحضـور]]*2</f>
         <v>2</v>
       </c>
     </row>
@@ -444,7 +440,6 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <f>Table1[[#This Row],[الحضـور]]*2</f>
         <v>2</v>
       </c>
     </row>

</xml_diff>